<commit_message>
He cambiado el metal del hidrógeno y le he puesto la tilde a oxígeno
</commit_message>
<xml_diff>
--- a/client/public/Hojas de Calculo/ElementosSinFormulas.xlsx
+++ b/client/public/Hojas de Calculo/ElementosSinFormulas.xlsx
@@ -82,6 +82,9 @@
     <t xml:space="preserve">-1,1</t>
   </si>
   <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
     <t xml:space="preserve">Litio</t>
   </si>
   <si>
@@ -269,9 +272,6 @@
   </si>
   <si>
     <t xml:space="preserve">-3,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false</t>
   </si>
   <si>
     <t xml:space="preserve">Galio</t>
@@ -607,20 +607,20 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I46" activeCellId="0" sqref="I46"/>
+      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -737,7 +737,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,10 +745,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>1</v>
@@ -774,10 +774,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>1</v>
@@ -803,10 +803,10 @@
         <v>37</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>1</v>
@@ -832,10 +832,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>1</v>
@@ -861,10 +861,10 @@
         <v>56</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>2</v>
@@ -879,7 +879,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>12</v>
@@ -890,10 +890,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>2</v>
@@ -908,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>12</v>
@@ -919,10 +919,10 @@
         <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>2</v>
@@ -937,7 +937,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>12</v>
@@ -948,10 +948,10 @@
         <v>38</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>2</v>
@@ -966,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>12</v>
@@ -977,10 +977,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>2</v>
@@ -995,7 +995,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>12</v>
@@ -1006,10 +1006,10 @@
         <v>88</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>2</v>
@@ -1024,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>12</v>
@@ -1035,13 +1035,13 @@
         <v>22</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>1</v>
@@ -1053,7 +1053,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>12</v>
@@ -1064,13 +1064,13 @@
         <v>24</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>2</v>
@@ -1082,7 +1082,7 @@
         <v>6</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>12</v>
@@ -1093,13 +1093,13 @@
         <v>25</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" s="4" t="n">
         <v>2</v>
@@ -1111,7 +1111,7 @@
         <v>7</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>12</v>
@@ -1122,13 +1122,13 @@
         <v>26</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E18" s="4" t="n">
         <v>2</v>
@@ -1140,7 +1140,7 @@
         <v>8</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>12</v>
@@ -1151,13 +1151,13 @@
         <v>27</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>1</v>
@@ -1169,7 +1169,7 @@
         <v>9</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>12</v>
@@ -1180,13 +1180,13 @@
         <v>28</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>1</v>
@@ -1198,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>12</v>
@@ -1209,13 +1209,13 @@
         <v>46</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>1</v>
@@ -1227,7 +1227,7 @@
         <v>10</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>12</v>
@@ -1238,13 +1238,13 @@
         <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>1</v>
@@ -1256,7 +1256,7 @@
         <v>10</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>12</v>
@@ -1267,13 +1267,13 @@
         <v>29</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E23" s="4" t="n">
         <v>2</v>
@@ -1285,7 +1285,7 @@
         <v>11</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>12</v>
@@ -1296,13 +1296,13 @@
         <v>79</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E24" s="4" t="n">
         <v>1</v>
@@ -1314,7 +1314,7 @@
         <v>11</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I24" s="0" t="s">
         <v>12</v>
@@ -1325,10 +1325,10 @@
         <v>47</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>1</v>
@@ -1343,7 +1343,7 @@
         <v>11</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>12</v>
@@ -1354,10 +1354,10 @@
         <v>48</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D26" s="3" t="n">
         <v>2</v>
@@ -1372,7 +1372,7 @@
         <v>12</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>12</v>
@@ -1383,10 +1383,10 @@
         <v>30</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>2</v>
@@ -1401,7 +1401,7 @@
         <v>12</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I27" s="0" t="s">
         <v>12</v>
@@ -1412,13 +1412,13 @@
         <v>80</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>1</v>
@@ -1430,7 +1430,7 @@
         <v>12</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>12</v>
@@ -1441,10 +1441,10 @@
         <v>13</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D29" s="3" t="n">
         <v>3</v>
@@ -1459,7 +1459,7 @@
         <v>13</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I29" s="0" t="s">
         <v>12</v>
@@ -1470,13 +1470,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E30" s="4" t="n">
         <v>1</v>
@@ -1488,10 +1488,10 @@
         <v>13</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1517,7 +1517,7 @@
         <v>13</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>12</v>
@@ -1549,7 +1549,7 @@
         <v>87</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,7 +1563,7 @@
         <v>89</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E33" s="4" t="n">
         <v>1</v>
@@ -1592,7 +1592,7 @@
         <v>91</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E34" s="4" t="n">
         <v>1</v>
@@ -1636,7 +1636,7 @@
         <v>87</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,7 +1665,7 @@
         <v>98</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,7 +1694,7 @@
         <v>98</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1723,7 +1723,7 @@
         <v>98</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1752,7 +1752,7 @@
         <v>106</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1781,7 +1781,7 @@
         <v>106</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,7 +1810,7 @@
         <v>106</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,7 +1839,7 @@
         <v>115</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,7 +1868,7 @@
         <v>115</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,7 +1897,7 @@
         <v>115</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1926,7 @@
         <v>115</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1953,7 +1953,7 @@
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">

</xml_diff>

<commit_message>
Se ha puesto la tilde ha oxígeno de forma definitiva
</commit_message>
<xml_diff>
--- a/client/public/Hojas de Calculo/ElementosSinFormulas.xlsx
+++ b/client/public/Hojas de Calculo/ElementosSinFormulas.xlsx
@@ -349,7 +349,7 @@
     <t xml:space="preserve">Grupo16</t>
   </si>
   <si>
-    <t xml:space="preserve">Oxigeno</t>
+    <t xml:space="preserve">Oxígeno</t>
   </si>
   <si>
     <t xml:space="preserve">O</t>
@@ -614,13 +614,13 @@
       <selection pane="bottomRight" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1953,7 +1953,7 @@
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">

</xml_diff>